<commit_message>
added example kid to the data file
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,43 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoanneMiao/Documents/CMCM Lab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbenton2\Documents\CMCM_lab\joanne_summer_research\CMCM-JM-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B9AC20-ACCA-0240-9AFC-B09F13326962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB838F1-00D3-48B9-A64D-F61BAA771D48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{A927A17E-28E2-084B-B43E-22E9E78CA587}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{58282CEB-ABC6-4F29-A274-B04900CD887C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>two_consistent_pairing</t>
+  </si>
+  <si>
+    <t>fam_order</t>
+  </si>
+  <si>
+    <t>fam_grouping</t>
+  </si>
+  <si>
+    <t>shape_order</t>
+  </si>
+  <si>
+    <t>test_condition</t>
+  </si>
+  <si>
+    <t>test_trial_order</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>test_choice_most_like</t>
+  </si>
+  <si>
+    <t>test_choice_least_like</t>
+  </si>
+  <si>
+    <t>pretest_choice_most_like</t>
+  </si>
+  <si>
+    <t>pretest_choice_least_like</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>age (year.month)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -379,16 +423,108 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECA2D6C-66B2-1848-BCB3-0F023C862C96}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44D092E-2B5E-4558-B708-F1E353401188}">
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>3.8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a fake kid as an example
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbenton2\Documents\CMCM_lab\joanne_summer_research\CMCM-JM-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB838F1-00D3-48B9-A64D-F61BAA771D48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FAE12D-663E-42B7-993E-EA3A7F9F6E95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{58282CEB-ABC6-4F29-A274-B04900CD887C}"/>
   </bookViews>
@@ -494,7 +494,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
docs reflect change in pretest and test Q formats
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoanneMiao/Desktop/CMCM JM Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB133E0-E631-6D4A-AA04-55A8896B7B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED255F06-D56D-7648-83EB-AA9E8B3B779C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{58282CEB-ABC6-4F29-A274-B04900CD887C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="3yr (current)" sheetId="4" r:id="rId1"/>
+    <sheet name="4yr" sheetId="2" r:id="rId2"/>
+    <sheet name="3yr (old)" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -115,13 +117,64 @@
   </si>
   <si>
     <t>did not answer test Qs, possible their choice of  blue in pretest Qs refer to zoom icon</t>
+  </si>
+  <si>
+    <t>pretest_choice_blue(like)_like_Q</t>
+  </si>
+  <si>
+    <t>pretest_choice_orange_like_Q</t>
+  </si>
+  <si>
+    <t>pretest_choice_blue(like)_not_like_Q</t>
+  </si>
+  <si>
+    <t>pretest_choice_orange_not_like_Q</t>
+  </si>
+  <si>
+    <t>test_choice_consistent(curvilinear)_like_Q</t>
+  </si>
+  <si>
+    <t>test_choice_consistent(curvilinear)_not_like_Q</t>
+  </si>
+  <si>
+    <t>test_choice_inconsistent(rectilinear)_like_Q</t>
+  </si>
+  <si>
+    <t>consent form</t>
+  </si>
+  <si>
+    <t>Luke's form</t>
+  </si>
+  <si>
+    <t>0 = wrong</t>
+  </si>
+  <si>
+    <t>1 = right</t>
+  </si>
+  <si>
+    <t>test_choice_inconsistent(rectilinear)_not_like_Q</t>
+  </si>
+  <si>
+    <t>kid was frustrated, irritated, and out of patience from beginning. They did not want to engage. Gave no's for all responses. Possible the answers are not serious</t>
+  </si>
+  <si>
+    <t>times_watched_test_videos_(min 2)</t>
+  </si>
+  <si>
+    <t>familiarization_video_repetitions</t>
+  </si>
+  <si>
+    <t>times_watched_test videos_(min 2)</t>
+  </si>
+  <si>
+    <t>familiarization_videos_repetitions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,8 +182,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +207,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -156,9 +253,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,11 +580,356 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83B9A72-F2BC-1946-917E-7D386FB1F6C5}">
+  <dimension ref="A1:T6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="31" customWidth="1"/>
+    <col min="12" max="12" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.1640625" customWidth="1"/>
+    <col min="14" max="14" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" customWidth="1"/>
+    <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="12">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
+        <v>3</v>
+      </c>
+      <c r="S2" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF326E0-2758-784C-9687-01B26BE43816}">
+  <dimension ref="A1:W6"/>
+  <sheetViews>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.33203125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="31" customWidth="1"/>
+    <col min="13" max="13" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.1640625" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.1640625" customWidth="1"/>
+    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4.7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="12">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+      <c r="P2" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <v>2</v>
+      </c>
+      <c r="T2" s="3">
+        <v>2</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="K6" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44D092E-2B5E-4558-B708-F1E353401188}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -589,176 +1042,176 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>3.8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>3.4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>2</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>3.3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>3.9</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>